<commit_message>
Se añadió algunos casos de uso
</commit_message>
<xml_diff>
--- a/Proyecto/Requerimientos.xlsx
+++ b/Proyecto/Requerimientos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304B7CA-2D02-4D65-9059-94531941F21D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C1020-5ED5-4D67-8AEA-DEF6D67517F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7840" yWindow="-320" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="91">
   <si>
     <t>ReqID</t>
   </si>
@@ -142,27 +142,15 @@
     <t>CU011</t>
   </si>
   <si>
-    <t>Autenticar</t>
-  </si>
-  <si>
     <t>Generar flujo de proceso de concertación</t>
   </si>
   <si>
     <t>Enviar Correo a Segmentos</t>
   </si>
   <si>
-    <t>Votar</t>
-  </si>
-  <si>
-    <t>Agregar mejora</t>
-  </si>
-  <si>
     <t>El sistema comenzara cuando el DNP genere un nuevo mecanismo de concertación abierto o cerrado.</t>
   </si>
   <si>
-    <t>Gestion de Propuestas</t>
-  </si>
-  <si>
     <t>El sistema con concertación abierto debe permitir recolectar ideas desde cada segmento.</t>
   </si>
   <si>
@@ -190,9 +178,6 @@
     <t>El sistema debe poder organizar y gestionar los documentos externos y anexos disponibles subidos con el fin de defender o justificar las propuestas.</t>
   </si>
   <si>
-    <t>Si el proceso de concertacion se crea de forma cerrada solo los usuarios con el rol de experto pueden generar propuestas.</t>
-  </si>
-  <si>
     <t>Solo se puede generar una propuesta por segmento.</t>
   </si>
   <si>
@@ -229,9 +214,6 @@
     <t>Solo un administrador puede seleccionar los usuarios que tendran el rol de experto y cada rol puede ver unicamente las propuestas correspondientes a si mismo.</t>
   </si>
   <si>
-    <t>DNP, Sistema, Usuario</t>
-  </si>
-  <si>
     <t>Segmento, Usuario</t>
   </si>
   <si>
@@ -239,13 +221,128 @@
   </si>
   <si>
     <t>Sistema, Segmento, Usuario</t>
+  </si>
+  <si>
+    <t>Votar una propuesta</t>
+  </si>
+  <si>
+    <t>Agregar mejora a propuesta</t>
+  </si>
+  <si>
+    <t>Crear tipos de votación</t>
+  </si>
+  <si>
+    <t>Crear usuarios</t>
+  </si>
+  <si>
+    <t>Crear roles</t>
+  </si>
+  <si>
+    <t>Crear segmentos</t>
+  </si>
+  <si>
+    <t>Crear sectores</t>
+  </si>
+  <si>
+    <t>Configurar acceso de sectores</t>
+  </si>
+  <si>
+    <t>CU012</t>
+  </si>
+  <si>
+    <t>Calificación de expertos</t>
+  </si>
+  <si>
+    <t>CU013</t>
+  </si>
+  <si>
+    <t>Procesar propuesta ganadora</t>
+  </si>
+  <si>
+    <t>CU014</t>
+  </si>
+  <si>
+    <t>Publicar resultado del proceso</t>
+  </si>
+  <si>
+    <t>CU015</t>
+  </si>
+  <si>
+    <t>Cargar archivo PDF</t>
+  </si>
+  <si>
+    <t>Cargar archivo video</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Concertacion abierta: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Las propuestas son dadas por los segmentos.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Concertacion cerrada:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Solo los usuarios con el rol de experto pueden generar propuestas.</t>
+    </r>
+  </si>
+  <si>
+    <t>DNP, Sistema, 
+Segmento, Usuario</t>
+  </si>
+  <si>
+    <t>Gestion de Propuestas (Abierto)</t>
+  </si>
+  <si>
+    <t>REQ12</t>
+  </si>
+  <si>
+    <t>Gestion de Propuestas (Cerrado)</t>
+  </si>
+  <si>
+    <t>El sistema con concertación cerrado debe permitir que un panel de expertos generen las propuestas.</t>
+  </si>
+  <si>
+    <t>El DNP genera el concepto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,16 +358,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -293,28 +409,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,346 +721,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="36.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.26953125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>56</v>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>48</v>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>50</v>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>52</v>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>54</v>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B27" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>